<commit_message>
Fixed missing ':class: table-wrap' in ui_elements.rst; new version of shortcut spreadsheet
</commit_message>
<xml_diff>
--- a/files/Shortcuts_for_Kdenlive.xlsx
+++ b/files/Shortcuts_for_Kdenlive.xlsx
@@ -1227,9 +1227,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1389,7 +1388,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1410,7 +1409,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1424,6 +1423,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1479,8 +1482,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FF272727"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1571,10 +1574,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H127"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1594,22 +1597,6 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="str">
-        <f aca="false">"    "</f>
-        <v>    </v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <f aca="false">"   "</f>
-        <v>   </v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <f aca="false">"*"</f>
-        <v>*</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <f aca="false">" - "</f>
-        <v>-</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -1632,12 +1619,7 @@
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B3 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C3 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D3</f>
-        <v>* - Action Name
-     - Shortcuts
-     - Description</v>
-      </c>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1655,11 +1637,11 @@
       <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="str">
+      <c r="H4" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B4 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C4 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D4</f>
-        <v>* - Add Clip to Selection
-     - :kbd:`Alt++`
-     - Adds the clip of the active track to the selection at playhead position..</v>
+        <v>Add Clip to Selection
+:kbd:`Alt++`
+Adds the clip of the active track to the selection at playhead position..</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1669,7 +1651,7 @@
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1678,11 +1660,11 @@
       <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1" t="str">
+      <c r="H5" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B5 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C5 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D5</f>
-        <v>* - Add Marker/Guide quickly
-     - :kbd:`Num+*`
-     - On Numlock pad: * adds a marker/guide</v>
+        <v>Add Marker/Guide quickly
+:kbd:`Num+*`
+On Numlock pad: * adds a marker/guide</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1701,11 +1683,11 @@
       <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="H6" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B6 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C6 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D6</f>
-        <v>* - Add Subtitle
-     - :kbd:`Shift+S`
-     - Adds a subtitle at playhead positon..</v>
+        <v>Add Subtitle
+:kbd:`Shift+S`
+Adds a subtitle at playhead positon..</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1715,18 +1697,18 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="H7" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B7 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C7 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D7</f>
-        <v>* - Add Transition to Selection
-     - :kbd:`Alt+Shift+ +`
-     -</v>
+        <v>Add Transition to Selection
+:kbd:`Alt+Shift+ +`
+</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1745,11 +1727,11 @@
       <c r="E8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="H8" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B8 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C8 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D8</f>
-        <v>* - Add/Remove Guide
-     - :kbd:`G`
-     - Adds a guide at playhead position..</v>
+        <v>Add/Remove Guide
+:kbd:`G`
+Adds a guide at playhead position..</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1766,11 +1748,11 @@
       <c r="E9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="H9" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B9 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C9 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D9</f>
-        <v>* - Collapse/Expand Item
-     - :kbd:`&lt;`
-     -</v>
+        <v>Collapse/Expand Item
+:kbd:`&lt;`
+</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1789,11 +1771,11 @@
       <c r="E10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="H10" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B10 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C10 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D10</f>
-        <v>* - Configure Kdenlive...
-     - :kbd:`Ctrl+Shift+,`
-     - Opens the configure window</v>
+        <v>Configure Kdenlive...
+:kbd:`Ctrl+Shift+,`
+Opens the configure window</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1812,11 +1794,11 @@
       <c r="E11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="H11" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B11 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C11 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D11</f>
-        <v>* - Configure Keyboard Shortcuts...
-     - :kbd:`Ctrl+Alt+,`
-     - Opens the shotcut window</v>
+        <v>Configure Keyboard Shortcuts...
+:kbd:`Ctrl+Alt+,`
+Opens the shotcut window</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="33.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1835,12 +1817,12 @@
       <c r="E12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="1" t="str">
+      <c r="H12" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B12 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C12 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D12</f>
-        <v>* - Copy
-     - :kbd:`Ctrl+C`
+        <v>Copy
+:kbd:`Ctrl+C`
 Alternate:  :kbd:`Ctrl+Ins`
-     - Current selection</v>
+Current selection</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1859,11 +1841,11 @@
       <c r="E13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="H13" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B13 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C13 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D13</f>
-        <v>* - Group Clips
-     - :kbd:`Ctrl+G`
-     - Current selection</v>
+        <v>Group Clips
+:kbd:`Ctrl+G`
+Current selection</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1882,11 +1864,11 @@
       <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="H14" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B14 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C14 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D14</f>
-        <v>* - Ungroup Clips
-     - :kbd:`Ctrl+Shift+G`
-     - Current selection</v>
+        <v>Ungroup Clips
+:kbd:`Ctrl+Shift+G`
+Current selection</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,11 +1887,11 @@
       <c r="E15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="H15" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B15 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C15 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D15</f>
-        <v>* - Cut All Clips
-     - :kbd:`Ctrl+Shift+R`
-     - Cuts all clips at playhead position. Except tracks which are locked.</v>
+        <v>Cut All Clips
+:kbd:`Ctrl+Shift+R`
+Cuts all clips at playhead position. Except tracks which are locked.</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1928,11 +1910,11 @@
       <c r="E16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="H16" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B16 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C16 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D16</f>
-        <v>* - Cut Clip
-     - :kbd:`Shift+R`
-     - Cuts the clip of the active track at playhead position.</v>
+        <v>Cut Clip
+:kbd:`Shift+R`
+Cuts the clip of the active track at playhead position.</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1949,11 +1931,11 @@
       <c r="E17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="H17" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B17 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C17 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D17</f>
-        <v>* - Delete Selected Item
-     - :kbd:`Del`
-     -</v>
+        <v>Delete Selected Item
+:kbd:`Del`
+</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1970,11 +1952,11 @@
       <c r="E18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="1" t="str">
+      <c r="H18" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B18 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C18 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D18</f>
-        <v>* - Deselect Clip
-     - :kbd:`-`
-     -</v>
+        <v>Deselect Clip
+:kbd:`-`
+</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1991,11 +1973,11 @@
       <c r="E19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="1" t="str">
+      <c r="H19" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B19 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C19 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D19</f>
-        <v>* - Deselect Transition
-     - :kbd:`Shift+-`
-     -</v>
+        <v>Deselect Transition
+:kbd:`Shift+-`
+</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2012,11 +1994,11 @@
       <c r="E20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="1" t="str">
+      <c r="H20" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B20 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C20 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D20</f>
-        <v>* - Extract Timeline Zone
-     - :kbd:`Shift+X`
-     -</v>
+        <v>Extract Timeline Zone
+:kbd:`Shift+X`
+</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2035,11 +2017,11 @@
       <c r="E21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="1" t="str">
+      <c r="H21" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B21 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C21 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D21</f>
-        <v>* - Find Action…
-     - :kbd:`Ctrl+Alt+I`
-     - Opens the action window. Only possible with this shortcut.</v>
+        <v>Find Action…
+:kbd:`Ctrl+Alt+I`
+Opens the action window. Only possible with this shortcut.</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2056,11 +2038,11 @@
       <c r="E22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H22" s="1" t="str">
+      <c r="H22" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B22 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C22 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D22</f>
-        <v>* - Focus Timecode
-     - :kbd:`=`
-     -</v>
+        <v>Focus Timecode
+:kbd:`=`
+</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2077,11 +2059,11 @@
       <c r="E23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="1" t="str">
+      <c r="H23" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B23 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C23 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D23</f>
-        <v>* - Full Screen Mode
-     - :kbd:`Ctrl+Shift+F`
-     -</v>
+        <v>Full Screen Mode
+:kbd:`Ctrl+Shift+F`
+</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,11 +2082,11 @@
       <c r="E24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="1" t="str">
+      <c r="H24" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B24 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C24 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D24</f>
-        <v>* - Grab Current Item
-     - :kbd:`Shift+G`
-     - Select a clip -&gt; :kbd:`Shift + G` -&gt; move the clip with .kbd:`left/right`</v>
+        <v>Grab Current Item
+:kbd:`Shift+G`
+Select a clip -&gt; :kbd:`Shift + G` -&gt; move the clip with .kbd:`left/right`</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2121,11 +2103,11 @@
       <c r="E25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="H25" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B25 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C25 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D25</f>
-        <v>* - Insert Clip Zone in Timeline
-     - :kbd:`V`
-     -</v>
+        <v>Insert Clip Zone in Timeline
+:kbd:`V`
+</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2144,11 +2126,11 @@
       <c r="E26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H26" s="1" t="str">
+      <c r="H26" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B26 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C26 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D26</f>
-        <v>* - Insert Zone in Project Bin
-     - :kbd:`Ctrl+I`
-     - Clip monitor</v>
+        <v>Insert Zone in Project Bin
+:kbd:`Ctrl+I`
+Clip monitor</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2165,11 +2147,11 @@
       <c r="E27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="1" t="str">
+      <c r="H27" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B27 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C27 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D27</f>
-        <v>* - Kdenlive Handbook
-     - :kbd:`F1`
-     -</v>
+        <v>Kdenlive Handbook
+:kbd:`F1`
+</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2186,11 +2168,11 @@
       <c r="E28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="1" t="str">
+      <c r="H28" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B28 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C28 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D28</f>
-        <v>* - Lift Timeline Zone
-     - :kbd:`Z`
-     -</v>
+        <v>Lift Timeline Zone
+:kbd:`Z`
+</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2209,11 +2191,11 @@
       <c r="E29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="1" t="str">
+      <c r="H29" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B29 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C29 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D29</f>
-        <v>* - Mix Clips
-     - :kbd:`U`
-     - Or double click. Play head must be on the end/begin of 2 clips. Creates a transition between 2 clips on the same track.</v>
+        <v>Mix Clips
+:kbd:`U`
+Or double click. Play head must be on the end/begin of 2 clips. Creates a transition between 2 clips on the same track. </v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2232,11 +2214,11 @@
       <c r="E30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="1" t="str">
+      <c r="H30" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B30 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C30 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D30</f>
-        <v>* - Multitrack View
-     - :kbd:`F12`
-     - :menuselection:`Tool -&gt; Multicam tool` must be disabled</v>
+        <v>Multitrack View
+:kbd:`F12`
+:menuselection:`Tool -&gt; Multicam tool` must be disabled</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2255,11 +2237,11 @@
       <c r="E31" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="1" t="str">
+      <c r="H31" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B31 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C31 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D31</f>
-        <v>* - Switch Monitor Fullscreen
-     - :kbd:`F11`
-     - Monitor</v>
+        <v>Switch Monitor Fullscreen
+:kbd:`F11`
+Monitor</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2275,14 +2257,14 @@
       <c r="D32" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H32" s="1" t="str">
+      <c r="H32" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B32 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C32 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D32</f>
-        <v>* - Align Playhead to Mouse Position
-     - :kbd:`P`
-     - Timeline</v>
+        <v>Align Playhead to Mouse Position
+:kbd:`P`
+Timeline</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2298,14 +2280,14 @@
       <c r="D33" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="1" t="str">
+      <c r="H33" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B33 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C33 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D33</f>
-        <v>* - Forward
-     - :kbd:`L`
-     - Playback</v>
+        <v>Forward
+:kbd:`L`
+Playback</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2321,14 +2303,14 @@
       <c r="D34" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="1" t="str">
+      <c r="H34" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B34 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C34 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D34</f>
-        <v>* - Forward 1 Frame
-     - :kbd:`Right`
-     - Playback</v>
+        <v>Forward 1 Frame
+:kbd:`Right`
+Playback</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2344,14 +2326,14 @@
       <c r="D35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="1" t="str">
+      <c r="H35" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B35 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C35 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D35</f>
-        <v>* - Forward 1 Second
-     - :kbd:`Shift+Right`
-     - Playback</v>
+        <v>Forward 1 Second
+:kbd:`Shift+Right`
+Playback</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2367,14 +2349,14 @@
       <c r="D36" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="1" t="str">
+      <c r="H36" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B36 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C36 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D36</f>
-        <v>* - Go to Clip End
-     - :kbd:`End`
-     - Timeline</v>
+        <v>Go to Clip End
+:kbd:`End`
+Timeline</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2390,14 +2372,14 @@
       <c r="D37" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H37" s="1" t="str">
+      <c r="H37" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B37 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C37 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D37</f>
-        <v>* - Go to Clip Start
-     - :kbd:`Home`
-     - Timeline</v>
+        <v>Go to Clip Start
+:kbd:`Home`
+Timeline</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2413,14 +2395,14 @@
       <c r="D38" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H38" s="1" t="str">
+      <c r="H38" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B38 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C38 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D38</f>
-        <v>* - Go to Next Guide
-     - :kbd:`Ctrl+Right`
-     - Timeline</v>
+        <v>Go to Next Guide
+:kbd:`Ctrl+Right`
+Timeline</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2436,14 +2418,14 @@
       <c r="D39" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H39" s="1" t="str">
+      <c r="H39" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B39 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C39 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D39</f>
-        <v>* - Go to Next Snap Point
-     - :kbd:`Alt+Right`
-     - Timeline</v>
+        <v>Go to Next Snap Point
+:kbd:`Alt+Right`
+Timeline</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2459,14 +2441,14 @@
       <c r="D40" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H40" s="1" t="str">
+      <c r="H40" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B40 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C40 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D40</f>
-        <v>* - Go to Previous Guide
-     - :kbd:`Ctrl+Left`
-     - Timeline</v>
+        <v>Go to Previous Guide
+:kbd:`Ctrl+Left`
+Timeline</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2482,14 +2464,14 @@
       <c r="D41" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H41" s="1" t="str">
+      <c r="H41" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B41 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C41 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D41</f>
-        <v>* - Go to Previous Snap Point
-     - :kbd:`Alt+Left`
-     - Timeline</v>
+        <v>Go to Previous Snap Point
+:kbd:`Alt+Left`
+Timeline</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2505,14 +2487,14 @@
       <c r="D42" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H42" s="1" t="str">
+      <c r="H42" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B42 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C42 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D42</f>
-        <v>* - Go to Project End
-     - :kbd:`Ctrl+End`
-     - Timeline</v>
+        <v>Go to Project End
+:kbd:`Ctrl+End`
+Timeline</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2528,14 +2510,14 @@
       <c r="D43" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H43" s="1" t="str">
+      <c r="H43" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B43 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C43 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D43</f>
-        <v>* - Go to Project Start
-     - :kbd:`Ctrl+Home`
-     - Timeline</v>
+        <v>Go to Project Start
+:kbd:`Ctrl+Home`
+Timeline</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2551,14 +2533,14 @@
       <c r="D44" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H44" s="1" t="str">
+      <c r="H44" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B44 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C44 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D44</f>
-        <v>* - Go to Zone End
-     - :kbd:`Shift+O`
-     - Timeline</v>
+        <v>Go to Zone End
+:kbd:`Shift+O`
+Timeline</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2574,14 +2556,14 @@
       <c r="D45" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H45" s="1" t="str">
+      <c r="H45" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B45 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C45 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D45</f>
-        <v>* - Go to Zone Start
-     - :kbd:`Shift+I`
-     - Timeline</v>
+        <v>Go to Zone Start
+:kbd:`Shift+I`
+Timeline</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2597,14 +2579,14 @@
       <c r="D46" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H46" s="1" t="str">
+      <c r="H46" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B46 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C46 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D46</f>
-        <v>* - Loop Zone
-     - :kbd:`Ctrl+Shift+Space`
-     - Playback</v>
+        <v>Loop Zone
+:kbd:`Ctrl+Shift+Space`
+Playback</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2620,14 +2602,14 @@
       <c r="D47" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H47" s="1" t="str">
+      <c r="H47" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B47 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C47 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D47</f>
-        <v>* - Pause
-     - :kbd:`K`
-     - Playback</v>
+        <v>Pause
+:kbd:`K`
+Playback</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2643,14 +2625,14 @@
       <c r="D48" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H48" s="1" t="str">
+      <c r="H48" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B48 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C48 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D48</f>
-        <v>* - Play
-     - :kbd:`Space`
-     - Playback</v>
+        <v>Play
+:kbd:`Space`
+Playback</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2666,14 +2648,14 @@
       <c r="D49" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H49" s="1" t="str">
+      <c r="H49" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B49 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C49 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D49</f>
-        <v>* - Play Zone
-     - :kbd:`Ctrl+Space`
-     - Playback</v>
+        <v>Play Zone
+:kbd:`Ctrl+Space`
+Playback</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2689,14 +2671,14 @@
       <c r="D50" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H50" s="1" t="str">
+      <c r="H50" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B50 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C50 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D50</f>
-        <v>* - Rewind
-     - :kbd:`J`
-     - Playback</v>
+        <v>Rewind
+:kbd:`J`
+Playback</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2712,14 +2694,14 @@
       <c r="D51" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H51" s="1" t="str">
+      <c r="H51" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B51 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C51 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D51</f>
-        <v>* - Rewind 1 Frame
-     - :kbd:`Left`
-     - Playback</v>
+        <v>Rewind 1 Frame
+:kbd:`Left`
+Playback</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2735,14 +2717,14 @@
       <c r="D52" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H52" s="1" t="str">
+      <c r="H52" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B52 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C52 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D52</f>
-        <v>* - Rewind 1 Second
-     - :kbd:`Shift+Left`
-     - Playback</v>
+        <v>Rewind 1 Second
+:kbd:`Shift+Left`
+Playback</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2758,14 +2740,14 @@
       <c r="D53" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H53" s="1" t="str">
+      <c r="H53" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B53 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C53 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D53</f>
-        <v>* - New
-     - :kbd:`Ctrl+N`
-     - Creates a new Kdenlive project</v>
+        <v>New
+:kbd:`Ctrl+N`
+Creates a new Kdenlive project</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2781,14 +2763,14 @@
       <c r="D54" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H54" s="1" t="str">
+      <c r="H54" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B54 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C54 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D54</f>
-        <v>* - Open...
-     - :kbd:`Ctrl+O`
-     - Opens a Kdenlive project</v>
+        <v>Open...
+:kbd:`Ctrl+O`
+Opens a Kdenlive project</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2805,11 +2787,11 @@
       <c r="E55" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H55" s="1" t="str">
+      <c r="H55" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B55 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C55 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D55</f>
-        <v>* - Overwrite Clip Zone in Timeline
-     - :kbd:`B`
-     -</v>
+        <v>Overwrite Clip Zone in Timeline
+:kbd:`B`
+</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,12 +2808,12 @@
       <c r="E56" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="1" t="str">
+      <c r="H56" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B56 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C56 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D56</f>
-        <v>* - Paste
-     - :kbd:`Ctrl+V`
+        <v>Paste
+:kbd:`Ctrl+V`
 Alternate:  :kbd:`Shift+Ins`
-     -</v>
+</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2847,14 +2829,14 @@
       <c r="D57" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H57" s="1" t="str">
+      <c r="H57" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B57 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C57 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D57</f>
-        <v>* - Quit
-     - :kbd:`Ctrl+Q`
-     - Exits Kdenlive</v>
+        <v>Quit
+:kbd:`Ctrl+Q`
+Exits Kdenlive</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2871,11 +2853,11 @@
       <c r="E58" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H58" s="1" t="str">
+      <c r="H58" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B58 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C58 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D58</f>
-        <v>* - Redo
-     - :kbd:`Ctrl+Shift+Z`
-     -</v>
+        <v>Redo
+:kbd:`Ctrl+Shift+Z`
+</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2892,11 +2874,11 @@
       <c r="E59" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H59" s="1" t="str">
+      <c r="H59" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B59 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C59 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D59</f>
-        <v>* - Rename...
-     - :kbd:`F2`
-     -</v>
+        <v>Rename...
+:kbd:`F2`
+</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2915,11 +2897,11 @@
       <c r="E60" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H60" s="1" t="str">
+      <c r="H60" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B60 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C60 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D60</f>
-        <v>* - Render…
-     - :kbd:`Ctrl+Return`
-     - Opens the Render window.</v>
+        <v>Render…
+:kbd:`Ctrl+Return`
+Opens the Render window.</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,11 +2920,11 @@
       <c r="E61" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H61" s="1" t="str">
+      <c r="H61" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B61 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C61 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D61</f>
-        <v>* - Resize Item End
-     - :kbd:`)`
-     - On active track: Cut and deletes the end of the clip at playhead position.</v>
+        <v>Resize Item End
+:kbd:`)`
+On active track: Cut and deletes the end of the clip at playhead position.</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,11 +2943,11 @@
       <c r="E62" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H62" s="1" t="str">
+      <c r="H62" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B62 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C62 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D62</f>
-        <v>* - Resize Item Start
-     - :kbd:`(`
-     - On active track: Cut and deletes the start of the clip at playhead position.</v>
+        <v>Resize Item Start
+:kbd:`(`
+On active track: Cut and deletes the start of the clip at playhead position.</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,14 +2963,14 @@
       <c r="D63" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H63" s="1" t="str">
+      <c r="H63" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B63 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C63 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D63</f>
-        <v>* - Save
-     - :kbd:`Ctrl+S`
-     - Saves the current state of the project</v>
+        <v>Save
+:kbd:`Ctrl+S`
+Saves the current state of the project</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,14 +2986,14 @@
       <c r="D64" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H64" s="1" t="str">
+      <c r="H64" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B64 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C64 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D64</f>
-        <v>* - Save As...
-     - :kbd:`Ctrl+Shift+S`
-     - Saves the current state of the project with the name of your choice</v>
+        <v>Save As...
+:kbd:`Ctrl+Shift+S`
+Saves the current state of the project with the name of your choice</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,11 +3010,11 @@
       <c r="E65" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="1" t="str">
+      <c r="H65" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B65 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C65 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D65</f>
-        <v>* - Select Clip
-     - :kbd:`+`
-     -</v>
+        <v>Select Clip
+:kbd:`+`
+</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3049,11 +3031,11 @@
       <c r="E66" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="1" t="str">
+      <c r="H66" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B66 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C66 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D66</f>
-        <v>* - Select Transition
-     - :kbd:`Shift+ +`
-     -</v>
+        <v>Select Transition
+:kbd:`Shift+ +`
+</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3070,11 +3052,11 @@
       <c r="E67" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="1" t="str">
+      <c r="H67" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B67 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C67 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D67</f>
-        <v>* - Set Zone In
-     - :kbd:`I`
-     -</v>
+        <v>Set Zone In
+:kbd:`I`
+</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3091,11 +3073,11 @@
       <c r="E68" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H68" s="1" t="str">
+      <c r="H68" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B68 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C68 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D68</f>
-        <v>* - Set Zone Out
-     - :kbd:`O`
-     -</v>
+        <v>Set Zone Out
+:kbd:`O`
+</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="31.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3114,11 +3096,11 @@
       <c r="E69" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H69" s="1" t="str">
+      <c r="H69" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B69 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C69 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D69</f>
-        <v>* - Show Menubar
-     - :kbd:`Ctrl+M`
-     - Show Menubar
+        <v>Show Menubar
+:kbd:`Ctrl+M`
+Show Menubar
 Shows the menubar again after it has been hidden</v>
       </c>
     </row>
@@ -3136,11 +3118,11 @@
       <c r="E70" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="1" t="str">
+      <c r="H70" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B70 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C70 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D70</f>
-        <v>* - Start Preview Render
-     - :kbd:`Shift+Return`
-     -</v>
+        <v>Start Preview Render
+:kbd:`Shift+Return`
+</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3159,11 +3141,11 @@
       <c r="E71" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H71" s="1" t="str">
+      <c r="H71" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B71 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C71 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D71</f>
-        <v>* - Switch Monitor
-     - :kbd:`T`
-     - Switch between clip monitor and project monitor (timeline)</v>
+        <v>Switch Monitor
+:kbd:`T`
+Switch between clip monitor and project monitor (timeline)</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3182,11 +3164,11 @@
       <c r="E72" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H72" s="1" t="str">
+      <c r="H72" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B72 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C72 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D72</f>
-        <v>* - Razor Tool
-     - :kbd:`X`
-     - Tools</v>
+        <v>Razor Tool
+:kbd:`X`
+Tools</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3205,11 +3187,11 @@
       <c r="E73" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H73" s="1" t="str">
+      <c r="H73" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B73 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C73 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D73</f>
-        <v>* - Selection Tool
-     - :kbd:`S`
-     - Tools</v>
+        <v>Selection Tool
+:kbd:`S`
+Tools</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3228,18 +3210,18 @@
       <c r="E74" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="1" t="str">
+      <c r="H74" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B74 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C74 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D74</f>
-        <v>* - Spacer Tool
-     - :kbd:`M`
-     - Tools</v>
+        <v>Spacer Tool
+:kbd:`M`
+Tools</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="13" t="s">
         <v>182</v>
       </c>
       <c r="C75" s="7" t="s">
@@ -3251,11 +3233,11 @@
       <c r="E75" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H75" s="1" t="str">
+      <c r="H75" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B75 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C75 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D75</f>
-        <v>* - Deselect
-     - :kbd:`Ctrl+Shift+A`
-     - Tracks</v>
+        <v>Deselect
+:kbd:`Ctrl+Shift+A`
+Tracks</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,11 +3256,11 @@
       <c r="E76" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H76" s="1" t="str">
+      <c r="H76" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B76 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C76 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D76</f>
-        <v>* - Select All
-     - :kbd:`Ctrl+A`
-     - Works in:
+        <v>Select All
+:kbd:`Ctrl+A`
+Works in:
 - Timeline
 - Project Bin
 - Titler</v>
@@ -3300,11 +3282,11 @@
       <c r="E77" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="1" t="str">
+      <c r="H77" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B77 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C77 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D77</f>
-        <v>* - Select Audio Track 1
-     - :kbd:`Alt+1`
-     - Tracks</v>
+        <v>Select Audio Track 1
+:kbd:`Alt+1`
+Tracks</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3323,11 +3305,11 @@
       <c r="E78" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="1" t="str">
+      <c r="H78" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B78 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C78 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D78</f>
-        <v>* - Select Audio Track 2
-     - :kbd:`Alt+2`
-     - Tracks</v>
+        <v>Select Audio Track 2
+:kbd:`Alt+2`
+Tracks</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3346,11 +3328,11 @@
       <c r="E79" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H79" s="1" t="str">
+      <c r="H79" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B79 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C79 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D79</f>
-        <v>* - Select Audio Track 3
-     - :kbd:`Alt+3`
-     - Tracks</v>
+        <v>Select Audio Track 3
+:kbd:`Alt+3`
+Tracks</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3369,11 +3351,11 @@
       <c r="E80" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H80" s="1" t="str">
+      <c r="H80" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B80 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C80 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D80</f>
-        <v>* - Select Audio Track 4
-     - :kbd:`Alt+4`
-     - Tracks</v>
+        <v>Select Audio Track 4
+:kbd:`Alt+4`
+Tracks</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3392,11 +3374,11 @@
       <c r="E81" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H81" s="1" t="str">
+      <c r="H81" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B81 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C81 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D81</f>
-        <v>* - Select Audio Track 5
-     - :kbd:`Alt+5`
-     - Tracks</v>
+        <v>Select Audio Track 5
+:kbd:`Alt+5`
+Tracks</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3415,11 +3397,11 @@
       <c r="E82" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H82" s="1" t="str">
+      <c r="H82" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B82 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C82 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D82</f>
-        <v>* - Select Audio Track 6
-     - :kbd:`Alt+6`
-     - Tracks</v>
+        <v>Select Audio Track 6
+:kbd:`Alt+6`
+Tracks</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3438,11 +3420,11 @@
       <c r="E83" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H83" s="1" t="str">
+      <c r="H83" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B83 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C83 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D83</f>
-        <v>* - Select Audio Track 7
-     - :kbd:`Alt+7`
-     - Tracks</v>
+        <v>Select Audio Track 7
+:kbd:`Alt+7`
+Tracks</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3461,11 +3443,11 @@
       <c r="E84" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H84" s="1" t="str">
+      <c r="H84" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B84 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C84 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D84</f>
-        <v>* - Select Audio Track 8
-     - :kbd:`Alt+8`
-     - Tracks</v>
+        <v>Select Audio Track 8
+:kbd:`Alt+8`
+Tracks</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3484,11 +3466,11 @@
       <c r="E85" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="1" t="str">
+      <c r="H85" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B85 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C85 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D85</f>
-        <v>* - Select Audio Track 9
-     - :kbd:`Alt+9`
-     - Tracks</v>
+        <v>Select Audio Track 9
+:kbd:`Alt+9`
+Tracks</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3507,11 +3489,11 @@
       <c r="E86" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H86" s="1" t="str">
+      <c r="H86" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B86 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C86 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D86</f>
-        <v>* - Select Target 1
-     - :kbd:`Ctrl+1`
-     - 3-point-editing</v>
+        <v>Select Target 1
+:kbd:`Ctrl+1`
+3-point-editing</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3530,11 +3512,11 @@
       <c r="E87" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H87" s="1" t="str">
+      <c r="H87" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B87 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C87 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D87</f>
-        <v>* - Select Target 2
-     - :kbd:`Ctrl+2`
-     - 3-point-editing</v>
+        <v>Select Target 2
+:kbd:`Ctrl+2`
+3-point-editing</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3553,11 +3535,11 @@
       <c r="E88" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H88" s="1" t="str">
+      <c r="H88" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B88 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C88 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D88</f>
-        <v>* - Select Target 3
-     - :kbd:`Ctrl+3`
-     - 3-point-editing</v>
+        <v>Select Target 3
+:kbd:`Ctrl+3`
+3-point-editing</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3576,11 +3558,11 @@
       <c r="E89" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H89" s="1" t="str">
+      <c r="H89" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B89 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C89 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D89</f>
-        <v>* - Select Target 4
-     - :kbd:`Ctrl+4`
-     - 3-point-editing</v>
+        <v>Select Target 4
+:kbd:`Ctrl+4`
+3-point-editing</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3599,11 +3581,11 @@
       <c r="E90" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H90" s="1" t="str">
+      <c r="H90" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B90 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C90 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D90</f>
-        <v>* - Select Target 5
-     - :kbd:`Ctrl+5`
-     - 3-point-editing</v>
+        <v>Select Target 5
+:kbd:`Ctrl+5`
+3-point-editing</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3622,11 +3604,11 @@
       <c r="E91" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H91" s="1" t="str">
+      <c r="H91" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B91 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C91 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D91</f>
-        <v>* - Select Target 6
-     - :kbd:`Ctrl+6`
-     - 3-point-editing</v>
+        <v>Select Target 6
+:kbd:`Ctrl+6`
+3-point-editing</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3645,11 +3627,11 @@
       <c r="E92" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H92" s="1" t="str">
+      <c r="H92" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B92 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C92 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D92</f>
-        <v>* - Select Target 7
-     - :kbd:`Ctrl+7`
-     - 3-point-editing</v>
+        <v>Select Target 7
+:kbd:`Ctrl+7`
+3-point-editing</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3668,11 +3650,11 @@
       <c r="E93" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H93" s="1" t="str">
+      <c r="H93" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B93 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C93 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D93</f>
-        <v>* - Select Target 8
-     - :kbd:`Ctrl+8`
-     - 3-point-editing</v>
+        <v>Select Target 8
+:kbd:`Ctrl+8`
+3-point-editing</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,11 +3673,11 @@
       <c r="E94" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H94" s="1" t="str">
+      <c r="H94" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B94 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C94 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D94</f>
-        <v>* - Select Target 9
-     - :kbd:`Ctrl+9`
-     - 3-point-editing</v>
+        <v>Select Target 9
+:kbd:`Ctrl+9`
+3-point-editing</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,11 +3696,11 @@
       <c r="E95" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H95" s="1" t="str">
+      <c r="H95" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B95 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C95 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D95</f>
-        <v>* - Select Video Track 1
-     - :kbd:`1`
-     - Track selection in general and for 3-point-editing|
+        <v>Select Video Track 1
+:kbd:`1`
+Track selection in general and for 3-point-editing|
 |
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
@@ -3739,11 +3721,11 @@
       <c r="E96" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H96" s="1" t="str">
+      <c r="H96" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B96 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C96 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D96</f>
-        <v>* - Select Video Track 2
-     - :kbd:`2`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 2
+:kbd:`2`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3763,11 +3745,11 @@
       <c r="E97" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H97" s="1" t="str">
+      <c r="H97" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B97 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C97 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D97</f>
-        <v>* - Select Video Track 3
-     - :kbd:`3`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 3
+:kbd:`3`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3787,11 +3769,11 @@
       <c r="E98" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H98" s="1" t="str">
+      <c r="H98" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B98 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C98 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D98</f>
-        <v>* - Select Video Track 4
-     - :kbd:`4`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 4
+:kbd:`4`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3811,11 +3793,11 @@
       <c r="E99" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H99" s="1" t="str">
+      <c r="H99" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B99 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C99 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D99</f>
-        <v>* - Select Video Track 5
-     - :kbd:`5`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 5
+:kbd:`5`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3835,11 +3817,11 @@
       <c r="E100" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H100" s="1" t="str">
+      <c r="H100" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B100 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C100 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D100</f>
-        <v>* - Select Video Track 6
-     - :kbd:`6`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 6
+:kbd:`6`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3859,11 +3841,11 @@
       <c r="E101" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H101" s="1" t="str">
+      <c r="H101" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B101 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C101 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D101</f>
-        <v>* - Select Video Track 7
-     - :kbd:`7`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 7
+:kbd:`7`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3883,11 +3865,11 @@
       <c r="E102" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H102" s="1" t="str">
+      <c r="H102" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B102 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C102 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D102</f>
-        <v>* - Select Video Track 8
-     - :kbd:`8`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 8
+:kbd:`8`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3907,11 +3889,11 @@
       <c r="E103" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="1" t="str">
+      <c r="H103" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B103 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C103 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D103</f>
-        <v>* - Select Video Track 9
-     - :kbd:`9`
-     - Track selection in general and for 3-point-editing
+        <v>Select Video Track 9
+:kbd:`9`
+Track selection in general and for 3-point-editing
 Multicam tool: You trim the clips in the desired track while the timeline is playing</v>
       </c>
     </row>
@@ -3931,11 +3913,11 @@
       <c r="E104" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H104" s="1" t="str">
+      <c r="H104" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B104 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C104 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D104</f>
-        <v>* - Switch All Tracks Active
-     - :kbd:`Alt+Shift+A`
-     - 3-point-editing</v>
+        <v>Switch All Tracks Active
+:kbd:`Alt+Shift+A`
+3-point-editing</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3954,11 +3936,11 @@
       <c r="E105" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H105" s="1" t="str">
+      <c r="H105" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B105 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C105 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D105</f>
-        <v>* - Switch Track Target Audio Stream
-     - :kbd:`'`
-     - Tracks</v>
+        <v>Switch Track Target Audio Stream
+:kbd:`'`
+Tracks</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3977,11 +3959,11 @@
       <c r="E106" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H106" s="1" t="str">
+      <c r="H106" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B106 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C106 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D106</f>
-        <v>* - Toggle All Track Lock
-     - :kbd:`Ctrl+Shift+L`
-     - Tracks</v>
+        <v>Toggle All Track Lock
+:kbd:`Ctrl+Shift+L`
+Tracks</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4000,11 +3982,11 @@
       <c r="E107" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H107" s="1" t="str">
+      <c r="H107" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B107 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C107 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D107</f>
-        <v>* - Toggle All Tracks Active
-     - :kbd:`Shift+A`
-     - 3-point-editing</v>
+        <v>Toggle All Tracks Active
+:kbd:`Shift+A`
+3-point-editing</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4023,11 +4005,11 @@
       <c r="E108" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H108" s="1" t="str">
+      <c r="H108" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B108 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C108 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D108</f>
-        <v>* - Toggle Track Active
-     - :kbd:`A`
-     - 3-point-editing
+        <v>Toggle Track Active
+:kbd:`A`
+3-point-editing
 Activate the track as a target with shortcut :kbd:`A` (this connects the track to the source)</v>
       </c>
     </row>
@@ -4047,11 +4029,11 @@
       <c r="E109" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H109" s="1" t="str">
+      <c r="H109" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B109 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C109 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D109</f>
-        <v>* - Toggle Track Disabled
-     - :kbd:`Shift+H`
-     - Tracks</v>
+        <v>Toggle Track Disabled
+:kbd:`Shift+H`
+Tracks</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4070,11 +4052,11 @@
       <c r="E110" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H110" s="1" t="str">
+      <c r="H110" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B110 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C110 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D110</f>
-        <v>* - Toggle Track Lock
-     - :kbd:`Shift+L`
-     - Tracks</v>
+        <v>Toggle Track Lock
+:kbd:`Shift+L`
+Tracks</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4093,11 +4075,11 @@
       <c r="E111" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H111" s="1" t="str">
+      <c r="H111" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B111 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C111 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D111</f>
-        <v>* - Toggle Track Target
-     - :kbd:`Shift+T`
-     - 3-point-editing
+        <v>Toggle Track Target
+:kbd:`Shift+T`
+3-point-editing
 Select a video or audio track in the timeline (up/down arrow key) and set it as source with :kbd:`Shift + T`.</v>
       </c>
     </row>
@@ -4115,11 +4097,11 @@
       <c r="E112" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H112" s="1" t="str">
+      <c r="H112" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B112 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C112 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D112</f>
-        <v>* - Undo
-     - :kbd:`Ctrl+Z`
-     -</v>
+        <v>Undo
+:kbd:`Ctrl+Z`
+</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4136,11 +4118,11 @@
       <c r="E113" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H113" s="1" t="str">
+      <c r="H113" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B113 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C113 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D113</f>
-        <v>* - Up
-     - :kbd:`Alt+Up`
-     -</v>
+        <v>Up
+:kbd:`Alt+Up`
+</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4157,11 +4139,11 @@
       <c r="E114" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H114" s="1" t="str">
+      <c r="H114" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B114 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C114 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D114</f>
-        <v>* - What's This?
-     - :kbd:`Shift+F1`
-     -</v>
+        <v>What's This?
+:kbd:`Shift+F1`
+</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,19 +4162,19 @@
       <c r="E115" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H115" s="1" t="str">
+      <c r="H115" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B115 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C115 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D115</f>
-        <v>* - Zoom In
-     - :kbd:`Ctrl+ +`
+        <v>Zoom In
+:kbd:`Ctrl+ +`
 Alternate: :kbd:`Ctrl+=`
 :kbd:`Ctrl+Mouse wheel`
-     - Works in Timeline only
+Works in Timeline only
 Works in:
 - Timeline
 - Clip Monitor
 - Project Monitor
 - Project Bin
-- effects keyframe pane</v>
+- effects keyframe pane </v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,18 +4193,18 @@
       <c r="E116" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H116" s="1" t="str">
+      <c r="H116" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B116 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C116 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D116</f>
-        <v>* - Zoom Out
-     - :kbd:`Ctrl+-`
+        <v>Zoom Out
+:kbd:`Ctrl+-`
 :kbd:`Ctrl+Mouse wheel`
-     - Works in Timeline only
+Works in Timeline only
 Works in:
 - Timeline
 - Clip Monitor
 - Project Monitor
 - Project Bin
-- effects keyframe pane</v>
+- effects keyframe pane </v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4235,18 +4217,18 @@
       <c r="C117" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D117" s="13" t="s">
+      <c r="D117" s="14" t="s">
         <v>277</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F117" s="7"/>
-      <c r="H117" s="1" t="str">
+      <c r="H117" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B117 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C117 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D117</f>
-        <v>* - Resize only audio or video part of a clip
-     - :kbd:`Shift+resize`
-     - Only possible with keyboard</v>
+        <v>Resize only audio or video part of a clip
+:kbd:`Shift+resize`
+Only possible with keyboard</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4259,18 +4241,18 @@
       <c r="C118" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="D118" s="13" t="s">
+      <c r="D118" s="14" t="s">
         <v>277</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F118" s="7"/>
-      <c r="H118" s="1" t="str">
+      <c r="H118" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B118 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C118 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D118</f>
-        <v>* - Move audio or video part to another track independently.
-     - :kbd:`Alt+move`
-     - Only possible with keyboard</v>
+        <v>Move audio or video part to another track independently.
+:kbd:`Alt+move`
+Only possible with keyboard</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="19.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4283,18 +4265,18 @@
       <c r="C119" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="D119" s="13" t="s">
+      <c r="D119" s="14" t="s">
         <v>277</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F119" s="7"/>
-      <c r="H119" s="1" t="str">
+      <c r="H119" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B119 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C119 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D119</f>
-        <v>* - Adjust the speed of a clip
-     - :kbd:`Ctrl+dragging`
-     - Only possible with keyboard</v>
+        <v>Adjust the speed of a clip
+:kbd:`Ctrl+dragging`
+Only possible with keyboard</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,21 +4289,21 @@
       <c r="C120" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D120" s="13" t="s">
+      <c r="D120" s="14" t="s">
         <v>277</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F120" s="7"/>
-      <c r="H120" s="1" t="str">
+      <c r="H120" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B120 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C120 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D120</f>
-        <v>* - Return from any tools back to Selection tool. 
-     - :kbd:`ESC`: 
-     - Only possible with keyboard</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>Return from any tools back to Selection tool. 
+:kbd:`ESC`: 
+Only possible with keyboard</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <v>121</v>
       </c>
@@ -4337,14 +4319,8 @@
       <c r="E121" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H121" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B121 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C121 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D121</f>
-        <v>* - Add text
-     - :kbd:`Alt+T`
-     - Click on the canvas to add text</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
         <v>122</v>
       </c>
@@ -4360,14 +4336,8 @@
       <c r="E122" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H122" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B122 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C122 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D122</f>
-        <v>* - Add rectangle
-     - :kbd:`Alt+R`
-     - Drag the mouse to draw a rectangle</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <v>123</v>
       </c>
@@ -4383,14 +4353,8 @@
       <c r="E123" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H123" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B123 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C123 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D123</f>
-        <v>* - Add ellipse
-     - :kbd:`Alt+E`
-     - Drag the mouse to draw a ellipse.</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
         <v>124</v>
       </c>
@@ -4406,14 +4370,8 @@
       <c r="E124" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H124" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B124 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C124 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D124</f>
-        <v>* - Insert an image
-     - :kbd:`Alt+I`
-     - Insert an image</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
         <v>125</v>
       </c>
@@ -4427,14 +4385,8 @@
       <c r="E125" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H125" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B125 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C125 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D125</f>
-        <v>* - Back to selection tool
-     - :kbd:`Alt+S`
-     -</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
         <v>126</v>
       </c>
@@ -4450,14 +4402,8 @@
       <c r="E126" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="H126" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B126 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C126 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D126</f>
-        <v>* - Move selected items vertical only.
-     - :kbd:`Shift`
-     - Hold :kbd:`Shift` moves selected items vertical only.</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
         <v>127</v>
       </c>
@@ -4472,12 +4418,6 @@
       </c>
       <c r="E127" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="H127" s="1" t="str">
-        <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B127 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C127 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D127</f>
-        <v>* - Move selected items horizontally only.
-     - :kbd:`Shift+Alt`
-     - Hold :kbd:`Shift + Alt` moves selected items horizontally only.</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,11 +4436,11 @@
       <c r="E128" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H128" s="1" t="str">
+      <c r="H128" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B128 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C128 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D128</f>
-        <v>* - Increment, Decrement
-     - :kbd:`Mouse wheel`
-     - Works in:
+        <v>Increment, Decrement
+:kbd:`Mouse wheel`
+Works in:
 - Timeline, scroll the timeline left/right
 - Timeline Ruler,  project monitor
 - Clip Monitor 
@@ -4522,11 +4462,11 @@
       <c r="E129" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="H129" s="1" t="str">
+      <c r="H129" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B129 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C129 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D129</f>
-        <v>* - Closing the extra bins
-     - :kbd:`Ctrl+w`
-     -</v>
+        <v>Closing the extra bins
+:kbd:`Ctrl+w`
+</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4545,11 +4485,11 @@
       <c r="E130" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H130" s="1" t="str">
+      <c r="H130" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B130 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C130 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D130</f>
-        <v>* - Playback clip
-     - :kbd:`Shift` and move the mouse left/right
-     - Inside the clip monitor</v>
+        <v>Playback clip
+:kbd:`Shift` and move the mouse left/right
+Inside the clip monitor</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4568,11 +4508,11 @@
       <c r="E131" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H131" s="1" t="str">
+      <c r="H131" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B131 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C131 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D131</f>
-        <v>* - Tracks resized simultaneously
-     - :kbd:`Shift+dragging`
-     - Either for video or audio tracks.</v>
+        <v>Tracks resized simultaneously
+:kbd:`Shift+dragging`
+Either for video or audio tracks.</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,11 +4531,11 @@
       <c r="E132" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H132" s="1" t="str">
+      <c r="H132" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B132 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C132 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D132</f>
-        <v>* - Tracks resized simultaneously to normal
-     - :kbd:`Shift+double click`
-     - Normalize track hight either for video or audio tracks.</v>
+        <v>Tracks resized simultaneously to normal
+:kbd:`Shift+double click`
+Normalize track hight either for video or audio tracks.</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,12 +4554,12 @@
       <c r="E133" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H133" s="1" t="str">
+      <c r="H133" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B133 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C133 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D133</f>
-        <v>* - Add to the selection
-     - :kbd:`Shift+left click`
+        <v>Add to the selection
+:kbd:`Shift+left click`
 :kbd:`shift+dragging`
-     - Timeline: adds clicked clips to the selection
+Timeline: adds clicked clips to the selection
 Timeline: adds multiple clips to the selection
 Titler: adds clicked clips to the selection
 Project Bin: adds all clips between already selected clip and clicked clip</v>
@@ -4641,11 +4581,11 @@
       <c r="E134" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H134" s="1" t="str">
+      <c r="H134" s="9" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B134 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C134 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D134</f>
-        <v>* - Add to the selection
-     - :kbd:`Ctrl+left click`
-     - Project Bin: adds clicked clips to the selection
+        <v>Add to the selection
+:kbd:`Ctrl+left click`
+Project Bin: adds clicked clips to the selection
 Effect: select keyframes</v>
       </c>
     </row>
@@ -4667,9 +4607,9 @@
       </c>
       <c r="H135" s="1" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B135 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C135 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D135</f>
-        <v>* - Slip multiple clips at once
-     - :kbd:`Shift+move`
-     - select all clips you want to slip with the selection tool using :kbd:`Shift` then enable the slip tool and go ahead…</v>
+        <v>Slip multiple clips at once
+:kbd:`Shift+move`
+select all clips you want to slip with the selection tool using :kbd:`Shift` then enable the slip tool and go ahead…</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,9 +4630,9 @@
       </c>
       <c r="H136" s="1" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B136 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C136 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D136</f>
-        <v>* - Slip a clip
-     - :kbd:`left/right`
-     - Slip can be done with the mouse, with the :kbd:`left/right` keys and with the buttons on the monitor toolbar.</v>
+        <v>Slip a clip
+:kbd:`left/right`
+Slip can be done with the mouse, with the :kbd:`left/right` keys and with the buttons on the monitor toolbar.</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4713,9 +4653,9 @@
       </c>
       <c r="H137" s="1" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B137 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C137 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D137</f>
-        <v>* - Double click
-     - :kbd:`double click`
-     - Edit bookmark
+        <v>Double click
+:kbd:`double click`
+Edit bookmark
 Project Bin: :kbd:`double click`on a clip shows properties
 Project Bin: :kbd:`double click`on an empty place opens `add clip or folder`
 Timeline: :kbd:`double click`a clip shows duration</v>
@@ -4737,21 +4677,21 @@
       </c>
       <c r="H138" s="1" t="str">
         <f aca="false">$G$1 &amp; $H$1 &amp; $I$1 &amp; B138 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; C138 &amp; CHAR(10) &amp; $F$1 &amp; $I$1 &amp; D138</f>
-        <v>* - Track selection
-     - :kbd:`up/down`
-     -</v>
+        <v>Track selection
+:kbd:`up/down`
+</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="14" t="s">
+      <c r="B140" s="15" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="C142" s="15" t="s">
+      <c r="C142" s="16" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4785,10 +4725,10 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H3:H127 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1:I127 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.78125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.76171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -4821,82 +4761,82 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>359</v>
       </c>
     </row>

</xml_diff>